<commit_message>
adicionando mais segundos pq o sistema esta travando muito
</commit_message>
<xml_diff>
--- a/CODIGOS.xlsx
+++ b/CODIGOS.xlsx
@@ -930,36 +930,71 @@
       <c r="A48" t="n">
         <v>23080</v>
       </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
         <v>23341</v>
       </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
         <v>23464</v>
       </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
         <v>23820</v>
       </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
         <v>24344</v>
       </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
         <v>24414</v>
       </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
           <t>024425CE</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
@@ -967,11 +1002,21 @@
       <c r="A55" t="n">
         <v>24876</v>
       </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
         <v>24932</v>
       </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -979,6 +1024,11 @@
           <t>025037CE</t>
         </is>
       </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -986,6 +1036,11 @@
           <t>025038CE</t>
         </is>
       </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -993,6 +1048,11 @@
           <t>025039CE</t>
         </is>
       </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -1000,6 +1060,11 @@
           <t>025041CE</t>
         </is>
       </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -1007,6 +1072,11 @@
           <t>025061CE</t>
         </is>
       </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -1014,6 +1084,11 @@
           <t>025062CE</t>
         </is>
       </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -1021,6 +1096,11 @@
           <t>025063CE</t>
         </is>
       </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -1028,11 +1108,21 @@
           <t>025072CE</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
           <t>025105CE</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
@@ -1040,6 +1130,11 @@
       <c r="A66" t="n">
         <v>25151</v>
       </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -1047,6 +1142,11 @@
           <t>025162CE</t>
         </is>
       </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -1054,6 +1154,11 @@
           <t>025165CE</t>
         </is>
       </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -1061,6 +1166,11 @@
           <t>025167CE</t>
         </is>
       </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -1068,11 +1178,21 @@
           <t>025168CE</t>
         </is>
       </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
           <t>026027CE</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
@@ -1080,16 +1200,31 @@
       <c r="A72" t="n">
         <v>26086</v>
       </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
         <v>26087</v>
       </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
           <t>026169CE</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
@@ -1097,11 +1232,21 @@
       <c r="A75" t="n">
         <v>26244</v>
       </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
           <t>026328ce</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
@@ -1109,21 +1254,41 @@
       <c r="A77" t="n">
         <v>26501</v>
       </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
         <v>26582</v>
       </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
         <v>26583</v>
       </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
           <t>026598CE</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
@@ -1131,11 +1296,21 @@
       <c r="A81" t="n">
         <v>26670</v>
       </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
           <t>027559CE</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
@@ -1143,36 +1318,71 @@
       <c r="A83" t="n">
         <v>27595</v>
       </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
         <v>27623</v>
       </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
         <v>27630</v>
       </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
         <v>27835</v>
       </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
         <v>27953</v>
       </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
         <v>28038</v>
       </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
         <v>28876</v>
       </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -1180,11 +1390,21 @@
           <t>028977CE</t>
         </is>
       </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
           <t>028978CE</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
@@ -1192,32 +1412,62 @@
       <c r="A92" t="n">
         <v>29014</v>
       </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
         <v>29414</v>
       </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
         <v>29451</v>
       </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
         <v>29454</v>
       </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
           <t>029493CE</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>LIDO</t>
         </is>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
         <v>29504</v>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>LIDO</t>
+        </is>
       </c>
     </row>
     <row r="98">

</xml_diff>